<commit_message>
invariants on attester merged and changed to current style invariant inv-dh-cmp-10 on section deleted invariant inv-dh-cmp-07 on authorRole deleted copyright updated to 2020 usage scenarios and implementation guidance updated use 1.1.1 of aubase for dependencyList.version in ig-advancecarerecords-1.jsonSet implementation guidance to "TBD" corrected some relative paths in invariants corrected description of invariant about profile reorder some invariants added invariant on attester.party
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/composition-acdcr-1.xlsx
+++ b/output/AdvanceCareRecords/composition-acdcr-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="418">
   <si>
     <t>Path</t>
   </si>
@@ -153,7 +153,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-03:If the author is a practitioner, the role shall be provided {(Composition.author.resolve() is Practitioner) implies Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-02:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-04:If and only if the author is a practitioner, the role shall be provided {author.resolve().where($this is Practitioner ).exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists()}inv-dh-cmp-05:If present, an authoring role shall at least have a reference that conforms to PractitionerRole with Practitioner with Mandatory Identifier or an identifier with at least a system and a value {extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1') or extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-cmp-03:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Document[classCode="DOC" and moodCode="EVN" and isNormalAct()]</t>
@@ -206,7 +206,7 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acdcr-1' {Composition.meta.profile.where($this='http://hl7.org.au/fhir/3.0/StructureDefinition/composition-acdcr-1').exists()}
+    <t xml:space="preserve">inv-dh-cmp-06:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acdcr-1' {profile.where($this='http://hl7.org.au/fhir/3.0/StructureDefinition/composition-acdcr-1').exists()}
 </t>
   </si>
   <si>
@@ -497,7 +497,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-04:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>informationRecipient</t>
@@ -511,10 +511,6 @@
   </si>
   <si>
     <t>A recipient who should receive a copy of the composition. A recipient is an entity to whom a copy of the composition is directed at the time of authoring of the composition.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Composition.modifierExtension</t>
@@ -657,7 +653,7 @@
     <t>Composition.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -738,7 +734,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -807,7 +803,7 @@
 </t>
   </si>
   <si>
-    <t>Legal attester</t>
+    <t>Legal Attester</t>
   </si>
   <si>
     <t>A participant who has attested to the accuracy of the composition/document.</t>
@@ -820,7 +816,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-inv-com-0:Related party and party shall not coexist {(attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists() and attester.party.exists()).not()}inv-dh-cmp-02:A legal attester shall have a party or a related party {Composition.attester.party.exists() or Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists()}</t>
+inv-com-0:Related party and party shall not coexist {(attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists() and attester.party.exists()).not()}inv-dh-cmp-08:A legal attester shall have a party or a related party that conforms to RelatedPerson with Mandatory Identifier {party.exists() xor extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1').exists()}inv-dh-cmp-07:If present, a party shall at least have a reference or an identifier with at least a system and a value {party.exists() implies (party.reference.exists() or party.identifier.where(system.count() + value.count() &gt; 1).exists())}</t>
   </si>
   <si>
     <t>.participation[typeCode="AUTHEN"].role[classCode="ASSIGNED"]</t>
@@ -848,10 +844,6 @@
     <t>A related person that attested this composition.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-05:A related party shall conform to RelatedPerson with Mandatory Identifier {Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1')}</t>
-  </si>
-  <si>
     <t>Composition.attester.modifierExtension</t>
   </si>
   <si>
@@ -916,7 +908,7 @@
     <t>Composition.attester.party</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -1124,7 +1116,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-11:An entry shall at least have a reference, an identifier or a display {entry.exists() implies section.entry.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
   </si>
   <si>
     <t>./outboundRelationship[typeCode="COMP" and isNormalActRelationship()]/target[moodCode="EVN" and classCode="DOCSECT" and isNormalAct]</t>
@@ -1277,7 +1269,7 @@
 </t>
   </si>
   <si>
-    <t>Persons acting as custodians (holders) of a patient's advance care directive</t>
+    <t>Entities acting as custodians (holders) of a patient's advance care directive</t>
   </si>
   <si>
     <t>A reference to the actual resource from which the narrative in the section is derived.</t>
@@ -3462,7 +3454,7 @@
         <v>152</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>39</v>
@@ -3476,7 +3468,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3502,10 +3494,10 @@
         <v>71</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>74</v>
@@ -3558,7 +3550,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3584,7 +3576,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3607,16 +3599,16 @@
         <v>51</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3666,7 +3658,7 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -3681,18 +3673,18 @@
         <v>39</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="AK20" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
         <v>169</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>170</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3718,16 +3710,16 @@
         <v>119</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>175</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>39</v>
@@ -3752,57 +3744,57 @@
         <v>39</v>
       </c>
       <c r="W21" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X21" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="X21" t="s" s="2">
+      <c r="Y21" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="Y21" t="s" s="2">
+      <c r="Z21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="Z21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE21" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="AF21" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
-        <v>179</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3825,94 +3817,94 @@
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>186</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W22" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="R22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W22" t="s" s="2">
+      <c r="X22" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="X22" t="s" s="2">
+      <c r="Y22" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="Y22" t="s" s="2">
+      <c r="Z22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE22" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="Z22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AK22" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>193</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3935,19 +3927,19 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>39</v>
@@ -3975,54 +3967,54 @@
         <v>109</v>
       </c>
       <c r="X23" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="Y23" t="s" s="2">
+      <c r="Z23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE23" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AF23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG23" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE23" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="AF23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG23" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ23" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4045,19 +4037,19 @@
         <v>51</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>39</v>
@@ -4106,7 +4098,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>50</v>
@@ -4121,18 +4113,18 @@
         <v>39</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AK24" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="AK24" t="s" s="2">
+      <c r="AL24" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>210</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4155,17 +4147,17 @@
         <v>51</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>214</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>39</v>
@@ -4214,7 +4206,7 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -4229,18 +4221,18 @@
         <v>39</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AK25" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="AK25" t="s" s="2">
+      <c r="AL25" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>218</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4263,19 +4255,19 @@
         <v>51</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>39</v>
@@ -4324,7 +4316,7 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>50</v>
@@ -4339,18 +4331,18 @@
         <v>39</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK26" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AK26" t="s" s="2">
+      <c r="AL26" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4373,17 +4365,17 @@
         <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>39</v>
@@ -4432,7 +4424,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>50</v>
@@ -4447,18 +4439,18 @@
         <v>39</v>
       </c>
       <c r="AJ27" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK27" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="AK27" t="s" s="2">
+      <c r="AL27" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4484,13 +4476,13 @@
         <v>64</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4540,7 +4532,7 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>50</v>
@@ -4555,10 +4547,10 @@
         <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK28" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>39</v>
@@ -4566,7 +4558,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4592,13 +4584,13 @@
         <v>119</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4624,49 +4616,49 @@
         <v>39</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X29" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="Y29" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y29" t="s" s="2">
+      <c r="Z29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Z29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>248</v>
-      </c>
       <c r="AK29" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>39</v>
@@ -4674,7 +4666,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4697,19 +4689,19 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>39</v>
@@ -4758,7 +4750,7 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4770,13 +4762,13 @@
         <v>39</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AJ30" t="s" s="2">
+      <c r="AK30" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>39</v>
@@ -4784,7 +4776,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4890,7 +4882,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4994,10 +4986,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="B33" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="B33" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>39</v>
@@ -5019,13 +5011,13 @@
         <v>39</v>
       </c>
       <c r="J33" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="K33" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="K33" t="s" s="2">
+      <c r="L33" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>263</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5088,7 +5080,7 @@
         <v>152</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>264</v>
+        <v>153</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>39</v>
@@ -5102,11 +5094,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5128,10 +5120,10 @@
         <v>71</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>74</v>
@@ -5184,7 +5176,7 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -5210,7 +5202,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5236,48 +5228,48 @@
         <v>119</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="Y35" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="R35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W35" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="X35" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="Y35" t="s" s="2">
-        <v>276</v>
-      </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
       </c>
@@ -5294,7 +5286,7 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>50</v>
@@ -5309,10 +5301,10 @@
         <v>39</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>39</v>
@@ -5320,7 +5312,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5343,17 +5335,17 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>39</v>
@@ -5402,7 +5394,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5417,10 +5409,10 @@
         <v>39</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>39</v>
@@ -5428,7 +5420,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5451,17 +5443,17 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>39</v>
@@ -5510,7 +5502,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5525,18 +5517,18 @@
         <v>39</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>292</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5559,19 +5551,19 @@
         <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>39</v>
@@ -5620,7 +5612,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5635,10 +5627,10 @@
         <v>39</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>39</v>
@@ -5646,7 +5638,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5669,16 +5661,16 @@
         <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5728,7 +5720,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5740,13 +5732,13 @@
         <v>39</v>
       </c>
       <c r="AI39" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>39</v>
@@ -5754,7 +5746,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5860,7 +5852,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5968,11 +5960,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -5994,10 +5986,10 @@
         <v>71</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>74</v>
@@ -6050,7 +6042,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6076,7 +6068,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6102,13 +6094,13 @@
         <v>119</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6134,49 +6126,49 @@
         <v>39</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X43" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="Y43" t="s" s="2">
+      <c r="AK43" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>39</v>
@@ -6184,7 +6176,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6207,13 +6199,13 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6264,7 +6256,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>50</v>
@@ -6279,10 +6271,10 @@
         <v>39</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>39</v>
@@ -6290,7 +6282,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6313,19 +6305,19 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>39</v>
@@ -6374,7 +6366,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6386,13 +6378,13 @@
         <v>39</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>39</v>
@@ -6400,7 +6392,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6506,7 +6498,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6614,11 +6606,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6640,10 +6632,10 @@
         <v>71</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>74</v>
@@ -6696,7 +6688,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6722,7 +6714,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6745,16 +6737,16 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6783,10 +6775,10 @@
         <v>109</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>39</v>
@@ -6804,7 +6796,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6819,10 +6811,10 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6830,7 +6822,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6853,13 +6845,13 @@
         <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6910,7 +6902,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6925,10 +6917,10 @@
         <v>39</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>39</v>
@@ -6936,7 +6928,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6959,13 +6951,13 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7016,7 +7008,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7031,7 +7023,7 @@
         <v>39</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>68</v>
@@ -7042,7 +7034,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7065,13 +7057,13 @@
         <v>39</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7122,7 +7114,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7134,13 +7126,13 @@
         <v>39</v>
       </c>
       <c r="AI52" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AK52" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>39</v>
@@ -7148,7 +7140,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7254,7 +7246,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7358,10 +7350,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>39</v>
@@ -7383,13 +7375,13 @@
         <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7452,7 +7444,7 @@
         <v>152</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>39</v>
@@ -7466,11 +7458,11 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7492,10 +7484,10 @@
         <v>71</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M56" t="s" s="2">
         <v>74</v>
@@ -7548,7 +7540,7 @@
         <v>39</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7574,11 +7566,11 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7600,23 +7592,23 @@
         <v>64</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P57" s="2"/>
       <c r="Q57" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R57" t="s" s="2">
         <v>39</v>
@@ -7658,7 +7650,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7673,10 +7665,10 @@
         <v>39</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7684,7 +7676,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7707,29 +7699,29 @@
         <v>39</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" t="s" s="2">
-        <v>374</v>
+        <v>39</v>
       </c>
       <c r="R58" t="s" s="2">
-        <v>39</v>
+        <v>372</v>
       </c>
       <c r="S58" t="s" s="2">
         <v>39</v>
@@ -7747,10 +7739,10 @@
         <v>109</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
@@ -7768,7 +7760,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7783,10 +7775,10 @@
         <v>39</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7794,7 +7786,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7820,13 +7812,13 @@
         <v>129</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -7876,7 +7868,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7885,16 +7877,16 @@
         <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7902,7 +7894,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7928,16 +7920,16 @@
         <v>119</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>39</v>
@@ -7962,57 +7954,57 @@
         <v>39</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="Y60" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="Z60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE60" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="AF60" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8035,19 +8027,19 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="M61" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>39</v>
@@ -8072,46 +8064,46 @@
         <v>39</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>68</v>
@@ -8122,7 +8114,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8145,16 +8137,16 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>402</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8204,7 +8196,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8213,16 +8205,16 @@
         <v>41</v>
       </c>
       <c r="AH62" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AK62" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="AI62" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>39</v>
@@ -8230,7 +8222,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8253,19 +8245,19 @@
         <v>39</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L63" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M63" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="N63" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>39</v>
@@ -8290,46 +8282,46 @@
         <v>39</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X63" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE63" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AF63" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG63" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH63" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AI63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ63" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="Y63" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="AF63" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG63" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH63" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="AI63" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ63" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="AK63" t="s" s="2">
         <v>68</v>
@@ -8340,7 +8332,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8366,13 +8358,13 @@
         <v>39</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8422,7 +8414,7 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8431,16 +8423,16 @@
         <v>41</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>39</v>

</xml_diff>